<commit_message>
updated user extractor name
</commit_message>
<xml_diff>
--- a/sheets/GetInAdjumaniUsers.xlsx
+++ b/sheets/GetInAdjumaniUsers.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Adjumani" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Adjumani!$F$1:$K$45</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Adjumani!$F$1:$K$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Adjumani!$F$1:$K$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Adjumani!$F$1:$K$45</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="120">
   <si>
     <t xml:space="preserve">First Name</t>
   </si>
@@ -385,9 +385,6 @@
   <si>
     <t xml:space="preserve">Amadrio</t>
   </si>
-  <si>
-    <t xml:space="preserve">Amadrio Scovia</t>
-  </si>
 </sst>
 </file>
 
@@ -601,8 +598,8 @@
   </sheetPr>
   <dimension ref="A1:AF1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2696,7 +2693,7 @@
         <v>119</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="C45" s="9" t="n">
         <v>789956252</v>
@@ -31389,7 +31386,7 @@
       <c r="AF1000" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="F1:K45"/>
+  <autoFilter ref="F1:K1"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>